<commit_message>
actualizacion de todos los modulos. correccion de bugs
</commit_message>
<xml_diff>
--- a/build/public/YVFMFrd9OgaAxgLci1fkiXge.xlsx
+++ b/build/public/YVFMFrd9OgaAxgLci1fkiXge.xlsx
@@ -1,23 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Angular\Citmatel\server\build\public\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20736" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2418" uniqueCount="530">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2407" uniqueCount="530">
   <si>
     <t>codped</t>
   </si>
@@ -1620,8 +1615,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1955,23 +1950,23 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:G473"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:B23"/>
+      <selection activeCell="B3" sqref="B3:G473"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1991,7 +1986,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:7">
       <c r="B4" t="s">
         <v>6</v>
       </c>
@@ -2011,7 +2006,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:7">
       <c r="B5" t="s">
         <v>10</v>
       </c>
@@ -2031,7 +2026,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:7">
       <c r="B6" t="s">
         <v>11</v>
       </c>
@@ -2051,7 +2046,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:7">
       <c r="B7" t="s">
         <v>12</v>
       </c>
@@ -2071,7 +2066,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:7">
       <c r="B8" t="s">
         <v>13</v>
       </c>
@@ -2091,7 +2086,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:7">
       <c r="B9" t="s">
         <v>14</v>
       </c>
@@ -2111,7 +2106,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:7">
       <c r="B10" t="s">
         <v>15</v>
       </c>
@@ -2131,7 +2126,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:7">
       <c r="B11" t="s">
         <v>16</v>
       </c>
@@ -2151,7 +2146,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:7">
       <c r="B12" t="s">
         <v>17</v>
       </c>
@@ -2171,7 +2166,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:7">
       <c r="B13" t="s">
         <v>18</v>
       </c>
@@ -2191,7 +2186,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:7">
       <c r="B14" t="s">
         <v>19</v>
       </c>
@@ -2211,7 +2206,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:7">
       <c r="B15" t="s">
         <v>20</v>
       </c>
@@ -2231,7 +2226,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:7">
       <c r="B16" t="s">
         <v>21</v>
       </c>
@@ -2251,7 +2246,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:7">
       <c r="B17" t="s">
         <v>22</v>
       </c>
@@ -2271,7 +2266,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:7">
       <c r="B18" t="s">
         <v>23</v>
       </c>
@@ -2291,7 +2286,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:7">
       <c r="B19" t="s">
         <v>24</v>
       </c>
@@ -2311,7 +2306,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:7">
       <c r="B20" t="s">
         <v>25</v>
       </c>
@@ -2331,7 +2326,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:7">
       <c r="B21" t="s">
         <v>26</v>
       </c>
@@ -2351,7 +2346,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:7">
       <c r="B22" t="s">
         <v>27</v>
       </c>
@@ -2371,7 +2366,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:7">
       <c r="B23" t="s">
         <v>28</v>
       </c>
@@ -2391,7 +2386,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:7">
       <c r="B24" t="s">
         <v>29</v>
       </c>
@@ -2411,7 +2406,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:7">
       <c r="B25" t="s">
         <v>30</v>
       </c>
@@ -2431,7 +2426,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:7">
       <c r="B26" t="s">
         <v>31</v>
       </c>
@@ -2451,7 +2446,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:7">
       <c r="B27" t="s">
         <v>32</v>
       </c>
@@ -2471,7 +2466,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:7">
       <c r="B28" t="s">
         <v>33</v>
       </c>
@@ -2491,7 +2486,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:7">
       <c r="B29" t="s">
         <v>34</v>
       </c>
@@ -2511,7 +2506,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:7">
       <c r="B30" t="s">
         <v>35</v>
       </c>
@@ -2531,7 +2526,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:7">
       <c r="B31" t="s">
         <v>36</v>
       </c>
@@ -2551,7 +2546,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:7">
       <c r="B32" t="s">
         <v>37</v>
       </c>
@@ -2571,7 +2566,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:7">
       <c r="B33" t="s">
         <v>38</v>
       </c>
@@ -2591,7 +2586,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:7">
       <c r="B34" t="s">
         <v>39</v>
       </c>
@@ -2611,7 +2606,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:7">
       <c r="B35" t="s">
         <v>40</v>
       </c>
@@ -2631,7 +2626,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:7">
       <c r="B36" t="s">
         <v>41</v>
       </c>
@@ -2651,7 +2646,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:7">
       <c r="B37" t="s">
         <v>42</v>
       </c>
@@ -2671,7 +2666,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:7">
       <c r="B38" t="s">
         <v>43</v>
       </c>
@@ -2691,7 +2686,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:7">
       <c r="B39" t="s">
         <v>44</v>
       </c>
@@ -2711,7 +2706,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:7">
       <c r="B40" t="s">
         <v>45</v>
       </c>
@@ -2731,7 +2726,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:7">
       <c r="B41" t="s">
         <v>46</v>
       </c>
@@ -2751,7 +2746,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:7">
       <c r="B42" t="s">
         <v>47</v>
       </c>
@@ -2771,7 +2766,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:7">
       <c r="B43" t="s">
         <v>48</v>
       </c>
@@ -2791,7 +2786,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:7">
       <c r="B44" t="s">
         <v>49</v>
       </c>
@@ -2811,7 +2806,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:7">
       <c r="B45" t="s">
         <v>50</v>
       </c>
@@ -2831,7 +2826,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:7">
       <c r="B46" t="s">
         <v>51</v>
       </c>
@@ -2851,7 +2846,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:7">
       <c r="B47" t="s">
         <v>52</v>
       </c>
@@ -2871,7 +2866,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:7">
       <c r="B48" t="s">
         <v>53</v>
       </c>
@@ -2891,7 +2886,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:7">
       <c r="B49" t="s">
         <v>54</v>
       </c>
@@ -2911,7 +2906,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:7">
       <c r="B50" t="s">
         <v>55</v>
       </c>
@@ -2931,7 +2926,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:7">
       <c r="B51" t="s">
         <v>56</v>
       </c>
@@ -2951,7 +2946,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:7">
       <c r="B52" t="s">
         <v>57</v>
       </c>
@@ -2971,7 +2966,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:7">
       <c r="B53" t="s">
         <v>58</v>
       </c>
@@ -2991,7 +2986,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:7">
       <c r="B54" t="s">
         <v>59</v>
       </c>
@@ -3011,7 +3006,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:7">
       <c r="B55" t="s">
         <v>60</v>
       </c>
@@ -3031,7 +3026,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:7">
       <c r="B56" t="s">
         <v>61</v>
       </c>
@@ -3051,7 +3046,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:7">
       <c r="B57" t="s">
         <v>62</v>
       </c>
@@ -3071,7 +3066,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:7">
       <c r="B58" t="s">
         <v>63</v>
       </c>
@@ -3091,7 +3086,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:7">
       <c r="B59" t="s">
         <v>64</v>
       </c>
@@ -3111,7 +3106,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:7">
       <c r="B60" t="s">
         <v>65</v>
       </c>
@@ -3131,7 +3126,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:7">
       <c r="B61" t="s">
         <v>66</v>
       </c>
@@ -3151,7 +3146,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:7">
       <c r="B62" t="s">
         <v>67</v>
       </c>
@@ -3171,7 +3166,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:7">
       <c r="B63" t="s">
         <v>68</v>
       </c>
@@ -3191,7 +3186,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:7">
       <c r="B64" t="s">
         <v>69</v>
       </c>
@@ -3211,7 +3206,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:7">
       <c r="B65" t="s">
         <v>70</v>
       </c>
@@ -3231,7 +3226,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:7">
       <c r="B66" t="s">
         <v>71</v>
       </c>
@@ -3251,7 +3246,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:7">
       <c r="B67" t="s">
         <v>72</v>
       </c>
@@ -3271,7 +3266,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="68" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:7">
       <c r="B68" t="s">
         <v>73</v>
       </c>
@@ -3291,7 +3286,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="69" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:7">
       <c r="B69" t="s">
         <v>74</v>
       </c>
@@ -3311,7 +3306,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="70" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:7">
       <c r="B70" t="s">
         <v>75</v>
       </c>
@@ -3331,7 +3326,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:7">
       <c r="B71" t="s">
         <v>76</v>
       </c>
@@ -3351,7 +3346,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="72" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:7">
       <c r="B72" t="s">
         <v>77</v>
       </c>
@@ -3371,7 +3366,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="73" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:7">
       <c r="B73" t="s">
         <v>78</v>
       </c>
@@ -3391,7 +3386,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:7">
       <c r="B74" t="s">
         <v>79</v>
       </c>
@@ -3411,7 +3406,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="75" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:7">
       <c r="B75" t="s">
         <v>80</v>
       </c>
@@ -3431,7 +3426,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="76" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:7">
       <c r="B76" t="s">
         <v>81</v>
       </c>
@@ -3451,7 +3446,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="77" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:7">
       <c r="B77" t="s">
         <v>82</v>
       </c>
@@ -3471,7 +3466,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="78" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:7">
       <c r="B78" t="s">
         <v>83</v>
       </c>
@@ -3491,7 +3486,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="79" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:7">
       <c r="B79" t="s">
         <v>84</v>
       </c>
@@ -3511,7 +3506,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="80" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:7">
       <c r="B80" t="s">
         <v>85</v>
       </c>
@@ -3531,7 +3526,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="81" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:7">
       <c r="B81" t="s">
         <v>86</v>
       </c>
@@ -3551,7 +3546,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="82" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:7">
       <c r="B82" t="s">
         <v>87</v>
       </c>
@@ -3571,7 +3566,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="83" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:7">
       <c r="B83" t="s">
         <v>88</v>
       </c>
@@ -3591,7 +3586,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="84" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:7">
       <c r="B84" t="s">
         <v>89</v>
       </c>
@@ -3611,7 +3606,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="85" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:7">
       <c r="B85" t="s">
         <v>90</v>
       </c>
@@ -3631,7 +3626,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="86" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:7">
       <c r="B86" t="s">
         <v>91</v>
       </c>
@@ -3651,7 +3646,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="87" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:7">
       <c r="B87" t="s">
         <v>92</v>
       </c>
@@ -3671,7 +3666,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="88" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:7">
       <c r="B88" t="s">
         <v>93</v>
       </c>
@@ -3691,7 +3686,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="89" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:7">
       <c r="B89" t="s">
         <v>94</v>
       </c>
@@ -3711,7 +3706,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="90" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:7">
       <c r="B90" t="s">
         <v>95</v>
       </c>
@@ -3731,7 +3726,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="91" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:7">
       <c r="B91" t="s">
         <v>96</v>
       </c>
@@ -3751,7 +3746,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:7">
       <c r="B92" t="s">
         <v>97</v>
       </c>
@@ -3771,7 +3766,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:7">
       <c r="B93" t="s">
         <v>98</v>
       </c>
@@ -3791,7 +3786,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="94" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:7">
       <c r="B94" t="s">
         <v>99</v>
       </c>
@@ -3811,7 +3806,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="95" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:7">
       <c r="B95" t="s">
         <v>100</v>
       </c>
@@ -3831,7 +3826,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:7">
       <c r="B96" t="s">
         <v>101</v>
       </c>
@@ -3851,7 +3846,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="97" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:7">
       <c r="B97" t="s">
         <v>102</v>
       </c>
@@ -3871,7 +3866,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="98" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:7">
       <c r="B98" t="s">
         <v>103</v>
       </c>
@@ -3891,7 +3886,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="99" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:7">
       <c r="B99" t="s">
         <v>104</v>
       </c>
@@ -3911,7 +3906,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="100" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:7">
       <c r="B100" t="s">
         <v>105</v>
       </c>
@@ -3931,7 +3926,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="101" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:7">
       <c r="B101" t="s">
         <v>106</v>
       </c>
@@ -3951,7 +3946,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="102" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:7">
       <c r="B102" t="s">
         <v>107</v>
       </c>
@@ -3971,7 +3966,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="103" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:7">
       <c r="B103" t="s">
         <v>108</v>
       </c>
@@ -3991,7 +3986,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="104" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:7">
       <c r="B104" t="s">
         <v>109</v>
       </c>
@@ -4011,7 +4006,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="105" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:7">
       <c r="B105" t="s">
         <v>110</v>
       </c>
@@ -4031,7 +4026,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="106" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:7">
       <c r="B106" t="s">
         <v>111</v>
       </c>
@@ -4051,7 +4046,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="107" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:7">
       <c r="B107" t="s">
         <v>112</v>
       </c>
@@ -4071,7 +4066,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="108" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:7">
       <c r="B108" t="s">
         <v>113</v>
       </c>
@@ -4091,7 +4086,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="109" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:7">
       <c r="B109" t="s">
         <v>114</v>
       </c>
@@ -4111,7 +4106,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="110" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:7">
       <c r="B110" t="s">
         <v>115</v>
       </c>
@@ -4131,7 +4126,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="111" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:7">
       <c r="B111" t="s">
         <v>116</v>
       </c>
@@ -4151,7 +4146,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="112" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:7">
       <c r="B112" t="s">
         <v>117</v>
       </c>
@@ -4171,7 +4166,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="113" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:7">
       <c r="B113" t="s">
         <v>118</v>
       </c>
@@ -4191,7 +4186,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="114" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:7">
       <c r="B114" t="s">
         <v>119</v>
       </c>
@@ -4211,7 +4206,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="115" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:7">
       <c r="B115" t="s">
         <v>120</v>
       </c>
@@ -4231,7 +4226,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="116" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:7">
       <c r="B116" t="s">
         <v>121</v>
       </c>
@@ -4251,7 +4246,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="117" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:7">
       <c r="B117" t="s">
         <v>122</v>
       </c>
@@ -4271,7 +4266,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="118" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:7">
       <c r="B118" t="s">
         <v>123</v>
       </c>
@@ -4291,7 +4286,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="119" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:7">
       <c r="B119" t="s">
         <v>124</v>
       </c>
@@ -4311,7 +4306,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="120" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:7">
       <c r="B120" t="s">
         <v>125</v>
       </c>
@@ -4331,7 +4326,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="121" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:7">
       <c r="B121" t="s">
         <v>126</v>
       </c>
@@ -4351,7 +4346,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="122" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:7">
       <c r="B122" t="s">
         <v>127</v>
       </c>
@@ -4371,7 +4366,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="123" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="123" spans="2:7">
       <c r="B123" t="s">
         <v>128</v>
       </c>
@@ -4391,7 +4386,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="124" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:7">
       <c r="B124" t="s">
         <v>129</v>
       </c>
@@ -4411,7 +4406,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="125" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:7">
       <c r="B125" t="s">
         <v>130</v>
       </c>
@@ -4431,7 +4426,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="126" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:7">
       <c r="B126" t="s">
         <v>131</v>
       </c>
@@ -4451,7 +4446,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="127" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:7">
       <c r="B127" t="s">
         <v>132</v>
       </c>
@@ -4471,7 +4466,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="128" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="128" spans="2:7">
       <c r="B128" t="s">
         <v>133</v>
       </c>
@@ -4491,7 +4486,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="129" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:7">
       <c r="B129" t="s">
         <v>134</v>
       </c>
@@ -4511,7 +4506,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="130" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:7">
       <c r="B130" t="s">
         <v>135</v>
       </c>
@@ -4531,7 +4526,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="131" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="131" spans="2:7">
       <c r="B131" t="s">
         <v>136</v>
       </c>
@@ -4551,7 +4546,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="132" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:7">
       <c r="B132" t="s">
         <v>137</v>
       </c>
@@ -4571,7 +4566,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="133" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:7">
       <c r="B133" t="s">
         <v>138</v>
       </c>
@@ -4591,7 +4586,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="134" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="134" spans="2:7">
       <c r="B134" t="s">
         <v>139</v>
       </c>
@@ -4611,7 +4606,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="135" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:7">
       <c r="B135" t="s">
         <v>140</v>
       </c>
@@ -4631,7 +4626,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="136" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:7">
       <c r="B136" t="s">
         <v>141</v>
       </c>
@@ -4651,7 +4646,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="137" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="137" spans="2:7">
       <c r="B137" t="s">
         <v>142</v>
       </c>
@@ -4671,7 +4666,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="138" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:7">
       <c r="B138" t="s">
         <v>143</v>
       </c>
@@ -4691,7 +4686,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="139" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:7">
       <c r="B139" t="s">
         <v>144</v>
       </c>
@@ -4711,7 +4706,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="140" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:7">
       <c r="B140" t="s">
         <v>145</v>
       </c>
@@ -4731,7 +4726,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="141" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:7">
       <c r="B141" t="s">
         <v>146</v>
       </c>
@@ -4751,7 +4746,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="142" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="142" spans="2:7">
       <c r="B142" t="s">
         <v>147</v>
       </c>
@@ -4771,7 +4766,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="143" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="143" spans="2:7">
       <c r="B143" t="s">
         <v>148</v>
       </c>
@@ -4791,7 +4786,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="144" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="144" spans="2:7">
       <c r="B144" t="s">
         <v>149</v>
       </c>
@@ -4811,7 +4806,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="145" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="145" spans="2:7">
       <c r="B145" t="s">
         <v>150</v>
       </c>
@@ -4831,7 +4826,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="146" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="146" spans="2:7">
       <c r="B146" t="s">
         <v>151</v>
       </c>
@@ -4851,7 +4846,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="147" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="147" spans="2:7">
       <c r="B147" t="s">
         <v>152</v>
       </c>
@@ -4871,7 +4866,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="148" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="148" spans="2:7">
       <c r="B148" t="s">
         <v>153</v>
       </c>
@@ -4891,7 +4886,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="149" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="149" spans="2:7">
       <c r="B149" t="s">
         <v>154</v>
       </c>
@@ -4911,7 +4906,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="150" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="150" spans="2:7">
       <c r="B150" t="s">
         <v>155</v>
       </c>
@@ -4931,7 +4926,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="151" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="151" spans="2:7">
       <c r="B151" t="s">
         <v>156</v>
       </c>
@@ -4951,7 +4946,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="152" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="152" spans="2:7">
       <c r="B152" t="s">
         <v>157</v>
       </c>
@@ -4971,7 +4966,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="153" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="153" spans="2:7">
       <c r="B153" t="s">
         <v>158</v>
       </c>
@@ -4991,7 +4986,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="154" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="154" spans="2:7">
       <c r="B154" t="s">
         <v>159</v>
       </c>
@@ -5011,7 +5006,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="155" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="155" spans="2:7">
       <c r="B155" t="s">
         <v>160</v>
       </c>
@@ -5031,7 +5026,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="156" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="156" spans="2:7">
       <c r="B156" t="s">
         <v>161</v>
       </c>
@@ -5051,7 +5046,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="157" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="157" spans="2:7">
       <c r="B157" t="s">
         <v>162</v>
       </c>
@@ -5071,7 +5066,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="158" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="158" spans="2:7">
       <c r="B158" t="s">
         <v>163</v>
       </c>
@@ -5091,7 +5086,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="159" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="159" spans="2:7">
       <c r="B159" t="s">
         <v>164</v>
       </c>
@@ -5111,7 +5106,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="160" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="160" spans="2:7">
       <c r="B160" t="s">
         <v>165</v>
       </c>
@@ -5131,7 +5126,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="161" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="161" spans="2:7">
       <c r="B161" t="s">
         <v>166</v>
       </c>
@@ -5151,7 +5146,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="162" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="162" spans="2:7">
       <c r="B162" t="s">
         <v>167</v>
       </c>
@@ -5171,7 +5166,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="163" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="163" spans="2:7">
       <c r="B163" t="s">
         <v>168</v>
       </c>
@@ -5191,7 +5186,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="164" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="164" spans="2:7">
       <c r="B164" t="s">
         <v>169</v>
       </c>
@@ -5211,7 +5206,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="165" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="165" spans="2:7">
       <c r="B165" t="s">
         <v>170</v>
       </c>
@@ -5231,7 +5226,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="166" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="166" spans="2:7">
       <c r="B166" t="s">
         <v>171</v>
       </c>
@@ -5251,7 +5246,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="167" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="167" spans="2:7">
       <c r="B167" t="s">
         <v>172</v>
       </c>
@@ -5271,7 +5266,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="168" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="168" spans="2:7">
       <c r="B168" t="s">
         <v>173</v>
       </c>
@@ -5291,7 +5286,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="169" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="169" spans="2:7">
       <c r="B169" t="s">
         <v>174</v>
       </c>
@@ -5311,7 +5306,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="170" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="170" spans="2:7">
       <c r="B170" t="s">
         <v>175</v>
       </c>
@@ -5331,7 +5326,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="171" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="171" spans="2:7">
       <c r="B171" t="s">
         <v>176</v>
       </c>
@@ -5351,7 +5346,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="172" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="172" spans="2:7">
       <c r="B172" t="s">
         <v>177</v>
       </c>
@@ -5371,7 +5366,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="173" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="173" spans="2:7">
       <c r="B173" t="s">
         <v>178</v>
       </c>
@@ -5391,7 +5386,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="174" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="174" spans="2:7">
       <c r="B174" t="s">
         <v>179</v>
       </c>
@@ -5411,7 +5406,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="175" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="175" spans="2:7">
       <c r="B175" t="s">
         <v>180</v>
       </c>
@@ -5431,7 +5426,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="176" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="176" spans="2:7">
       <c r="B176" t="s">
         <v>181</v>
       </c>
@@ -5451,7 +5446,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="177" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="177" spans="2:7">
       <c r="B177" t="s">
         <v>182</v>
       </c>
@@ -5471,7 +5466,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="178" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="178" spans="2:7">
       <c r="B178" t="s">
         <v>183</v>
       </c>
@@ -5491,7 +5486,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="179" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="179" spans="2:7">
       <c r="B179" t="s">
         <v>184</v>
       </c>
@@ -5511,7 +5506,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="180" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="180" spans="2:7">
       <c r="B180" t="s">
         <v>185</v>
       </c>
@@ -5531,7 +5526,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="181" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="181" spans="2:7">
       <c r="B181" t="s">
         <v>186</v>
       </c>
@@ -5551,7 +5546,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="182" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="182" spans="2:7">
       <c r="B182" t="s">
         <v>187</v>
       </c>
@@ -5571,7 +5566,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="183" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="183" spans="2:7">
       <c r="B183" t="s">
         <v>188</v>
       </c>
@@ -5591,7 +5586,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="184" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="184" spans="2:7">
       <c r="B184" t="s">
         <v>189</v>
       </c>
@@ -5611,7 +5606,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="185" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="185" spans="2:7">
       <c r="B185" t="s">
         <v>190</v>
       </c>
@@ -5631,7 +5626,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="186" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="186" spans="2:7">
       <c r="B186" t="s">
         <v>191</v>
       </c>
@@ -5651,7 +5646,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="187" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="187" spans="2:7">
       <c r="B187" t="s">
         <v>192</v>
       </c>
@@ -5671,7 +5666,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="188" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="188" spans="2:7">
       <c r="B188" t="s">
         <v>193</v>
       </c>
@@ -5691,7 +5686,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="189" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="189" spans="2:7">
       <c r="B189" t="s">
         <v>194</v>
       </c>
@@ -5711,7 +5706,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="190" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="190" spans="2:7">
       <c r="B190" t="s">
         <v>195</v>
       </c>
@@ -5731,7 +5726,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="191" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="191" spans="2:7">
       <c r="B191" t="s">
         <v>196</v>
       </c>
@@ -5751,7 +5746,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="192" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="192" spans="2:7">
       <c r="B192" t="s">
         <v>197</v>
       </c>
@@ -5771,7 +5766,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="193" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="193" spans="2:7">
       <c r="B193" t="s">
         <v>198</v>
       </c>
@@ -5791,7 +5786,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="194" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="194" spans="2:7">
       <c r="B194" t="s">
         <v>199</v>
       </c>
@@ -5811,7 +5806,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="195" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="195" spans="2:7">
       <c r="B195" t="s">
         <v>200</v>
       </c>
@@ -5831,7 +5826,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="196" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="196" spans="2:7">
       <c r="B196" t="s">
         <v>201</v>
       </c>
@@ -5851,7 +5846,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="197" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="197" spans="2:7">
       <c r="B197" t="s">
         <v>202</v>
       </c>
@@ -5871,7 +5866,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="198" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="198" spans="2:7">
       <c r="B198" t="s">
         <v>203</v>
       </c>
@@ -5891,7 +5886,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="199" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="199" spans="2:7">
       <c r="B199" t="s">
         <v>204</v>
       </c>
@@ -5911,7 +5906,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="200" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="200" spans="2:7">
       <c r="B200" t="s">
         <v>205</v>
       </c>
@@ -5931,7 +5926,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="201" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="201" spans="2:7">
       <c r="B201" t="s">
         <v>206</v>
       </c>
@@ -5951,7 +5946,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="202" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="202" spans="2:7">
       <c r="B202" t="s">
         <v>207</v>
       </c>
@@ -5971,7 +5966,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="203" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="203" spans="2:7">
       <c r="B203" t="s">
         <v>208</v>
       </c>
@@ -5991,7 +5986,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="204" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="204" spans="2:7">
       <c r="B204" t="s">
         <v>209</v>
       </c>
@@ -6011,7 +6006,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="205" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="205" spans="2:7">
       <c r="B205" t="s">
         <v>210</v>
       </c>
@@ -6031,7 +6026,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="206" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="206" spans="2:7">
       <c r="B206" t="s">
         <v>211</v>
       </c>
@@ -6051,7 +6046,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="207" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="207" spans="2:7">
       <c r="B207" t="s">
         <v>212</v>
       </c>
@@ -6071,7 +6066,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="208" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="208" spans="2:7">
       <c r="B208" t="s">
         <v>213</v>
       </c>
@@ -6091,7 +6086,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="209" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="209" spans="2:7">
       <c r="B209" t="s">
         <v>214</v>
       </c>
@@ -6111,7 +6106,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="210" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="210" spans="2:7">
       <c r="B210" t="s">
         <v>215</v>
       </c>
@@ -6131,7 +6126,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="211" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="211" spans="2:7">
       <c r="B211" t="s">
         <v>216</v>
       </c>
@@ -6151,7 +6146,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="212" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="212" spans="2:7">
       <c r="B212" t="s">
         <v>217</v>
       </c>
@@ -6171,7 +6166,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="213" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="213" spans="2:7">
       <c r="B213" t="s">
         <v>218</v>
       </c>
@@ -6191,7 +6186,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="214" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="214" spans="2:7">
       <c r="B214" t="s">
         <v>219</v>
       </c>
@@ -6211,7 +6206,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="215" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="215" spans="2:7">
       <c r="B215" t="s">
         <v>220</v>
       </c>
@@ -6231,7 +6226,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="216" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="216" spans="2:7">
       <c r="B216" t="s">
         <v>221</v>
       </c>
@@ -6251,7 +6246,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="217" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="217" spans="2:7">
       <c r="B217" t="s">
         <v>222</v>
       </c>
@@ -6271,7 +6266,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="218" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="218" spans="2:7">
       <c r="B218" t="s">
         <v>223</v>
       </c>
@@ -6291,7 +6286,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="219" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="219" spans="2:7">
       <c r="B219" t="s">
         <v>224</v>
       </c>
@@ -6311,7 +6306,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="220" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="220" spans="2:7">
       <c r="B220" t="s">
         <v>225</v>
       </c>
@@ -6331,7 +6326,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="221" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="221" spans="2:7">
       <c r="B221" t="s">
         <v>226</v>
       </c>
@@ -6351,7 +6346,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="222" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="222" spans="2:7">
       <c r="B222" t="s">
         <v>227</v>
       </c>
@@ -6371,7 +6366,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="223" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="223" spans="2:7">
       <c r="B223" t="s">
         <v>228</v>
       </c>
@@ -6391,7 +6386,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="224" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="224" spans="2:7">
       <c r="B224" t="s">
         <v>229</v>
       </c>
@@ -6411,7 +6406,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="225" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="225" spans="2:7">
       <c r="B225" t="s">
         <v>230</v>
       </c>
@@ -6431,7 +6426,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="226" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="226" spans="2:7">
       <c r="B226" t="s">
         <v>231</v>
       </c>
@@ -6451,7 +6446,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="227" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="227" spans="2:7">
       <c r="B227" t="s">
         <v>232</v>
       </c>
@@ -6471,7 +6466,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="228" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="228" spans="2:7">
       <c r="B228" t="s">
         <v>233</v>
       </c>
@@ -6491,7 +6486,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="229" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="229" spans="2:7">
       <c r="B229" t="s">
         <v>234</v>
       </c>
@@ -6511,7 +6506,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="230" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="230" spans="2:7">
       <c r="B230" t="s">
         <v>235</v>
       </c>
@@ -6531,7 +6526,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="231" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="231" spans="2:7">
       <c r="B231" t="s">
         <v>236</v>
       </c>
@@ -6551,7 +6546,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="232" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="232" spans="2:7">
       <c r="B232" t="s">
         <v>237</v>
       </c>
@@ -6571,7 +6566,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="233" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="233" spans="2:7">
       <c r="B233" t="s">
         <v>238</v>
       </c>
@@ -6591,7 +6586,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="234" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="234" spans="2:7">
       <c r="B234" t="s">
         <v>239</v>
       </c>
@@ -6611,7 +6606,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="235" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="235" spans="2:7">
       <c r="B235" t="s">
         <v>240</v>
       </c>
@@ -6631,7 +6626,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="236" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="236" spans="2:7">
       <c r="B236" t="s">
         <v>241</v>
       </c>
@@ -6651,7 +6646,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="237" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="237" spans="2:7">
       <c r="B237" t="s">
         <v>242</v>
       </c>
@@ -6671,7 +6666,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="238" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="238" spans="2:7">
       <c r="B238" t="s">
         <v>243</v>
       </c>
@@ -6691,7 +6686,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="239" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="239" spans="2:7">
       <c r="B239" t="s">
         <v>244</v>
       </c>
@@ -6711,7 +6706,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="240" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="240" spans="2:7">
       <c r="B240" t="s">
         <v>245</v>
       </c>
@@ -6731,7 +6726,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="241" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="241" spans="2:7">
       <c r="B241" t="s">
         <v>246</v>
       </c>
@@ -6751,7 +6746,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="242" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="242" spans="2:7">
       <c r="B242" t="s">
         <v>247</v>
       </c>
@@ -6771,7 +6766,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="243" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="243" spans="2:7">
       <c r="B243" t="s">
         <v>248</v>
       </c>
@@ -6791,7 +6786,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="244" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="244" spans="2:7">
       <c r="B244" t="s">
         <v>249</v>
       </c>
@@ -6811,7 +6806,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="245" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="245" spans="2:7">
       <c r="B245" t="s">
         <v>250</v>
       </c>
@@ -6831,7 +6826,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="246" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="246" spans="2:7">
       <c r="B246" t="s">
         <v>251</v>
       </c>
@@ -6851,7 +6846,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="247" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="247" spans="2:7">
       <c r="B247" t="s">
         <v>252</v>
       </c>
@@ -6871,7 +6866,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="248" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="248" spans="2:7">
       <c r="B248" t="s">
         <v>253</v>
       </c>
@@ -6891,7 +6886,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="249" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="249" spans="2:7">
       <c r="B249" t="s">
         <v>254</v>
       </c>
@@ -6911,7 +6906,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="250" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="250" spans="2:7">
       <c r="B250" t="s">
         <v>255</v>
       </c>
@@ -6931,7 +6926,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="251" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="251" spans="2:7">
       <c r="B251" t="s">
         <v>256</v>
       </c>
@@ -6951,7 +6946,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="252" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="252" spans="2:7">
       <c r="B252" t="s">
         <v>257</v>
       </c>
@@ -6971,7 +6966,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="253" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="253" spans="2:7">
       <c r="B253" t="s">
         <v>258</v>
       </c>
@@ -6991,7 +6986,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="254" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="254" spans="2:7">
       <c r="B254" t="s">
         <v>259</v>
       </c>
@@ -7011,7 +7006,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="255" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="255" spans="2:7">
       <c r="B255" t="s">
         <v>260</v>
       </c>
@@ -7031,7 +7026,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="256" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="256" spans="2:7">
       <c r="B256" t="s">
         <v>261</v>
       </c>
@@ -7051,7 +7046,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="257" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="257" spans="2:7">
       <c r="B257" t="s">
         <v>262</v>
       </c>
@@ -7071,7 +7066,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="258" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="258" spans="2:7">
       <c r="B258" t="s">
         <v>263</v>
       </c>
@@ -7091,7 +7086,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="259" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="259" spans="2:7">
       <c r="B259" t="s">
         <v>264</v>
       </c>
@@ -7111,7 +7106,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="260" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="260" spans="2:7">
       <c r="B260" t="s">
         <v>265</v>
       </c>
@@ -7131,7 +7126,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="261" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="261" spans="2:7">
       <c r="B261" t="s">
         <v>266</v>
       </c>
@@ -7151,7 +7146,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="262" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="262" spans="2:7">
       <c r="B262" t="s">
         <v>267</v>
       </c>
@@ -7171,7 +7166,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="263" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="263" spans="2:7">
       <c r="B263" t="s">
         <v>268</v>
       </c>
@@ -7191,7 +7186,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="264" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="264" spans="2:7">
       <c r="B264" t="s">
         <v>269</v>
       </c>
@@ -7211,7 +7206,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="265" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="265" spans="2:7">
       <c r="B265" t="s">
         <v>270</v>
       </c>
@@ -7231,7 +7226,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="266" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="266" spans="2:7">
       <c r="B266" t="s">
         <v>271</v>
       </c>
@@ -7251,7 +7246,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="267" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="267" spans="2:7">
       <c r="B267" t="s">
         <v>272</v>
       </c>
@@ -7271,7 +7266,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="268" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="268" spans="2:7">
       <c r="B268" t="s">
         <v>273</v>
       </c>
@@ -7291,7 +7286,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="269" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="269" spans="2:7">
       <c r="B269" t="s">
         <v>274</v>
       </c>
@@ -7311,7 +7306,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="270" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="270" spans="2:7">
       <c r="B270" t="s">
         <v>275</v>
       </c>
@@ -7331,7 +7326,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="271" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="271" spans="2:7">
       <c r="B271" t="s">
         <v>276</v>
       </c>
@@ -7351,7 +7346,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="272" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="272" spans="2:7">
       <c r="B272" t="s">
         <v>277</v>
       </c>
@@ -7371,7 +7366,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="273" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="273" spans="2:7">
       <c r="B273" t="s">
         <v>278</v>
       </c>
@@ -7391,7 +7386,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="274" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="274" spans="2:7">
       <c r="B274" t="s">
         <v>279</v>
       </c>
@@ -7411,7 +7406,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="275" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="275" spans="2:7">
       <c r="B275" t="s">
         <v>280</v>
       </c>
@@ -7431,7 +7426,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="276" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="276" spans="2:7">
       <c r="B276" t="s">
         <v>281</v>
       </c>
@@ -7451,7 +7446,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="277" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="277" spans="2:7">
       <c r="B277" t="s">
         <v>282</v>
       </c>
@@ -7471,7 +7466,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="278" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="278" spans="2:7">
       <c r="B278" t="s">
         <v>283</v>
       </c>
@@ -7491,7 +7486,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="279" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="279" spans="2:7">
       <c r="B279" t="s">
         <v>284</v>
       </c>
@@ -7511,7 +7506,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="280" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="280" spans="2:7">
       <c r="B280" t="s">
         <v>285</v>
       </c>
@@ -7531,7 +7526,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="281" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="281" spans="2:7">
       <c r="B281" t="s">
         <v>286</v>
       </c>
@@ -7551,7 +7546,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="282" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="282" spans="2:7">
       <c r="B282" t="s">
         <v>287</v>
       </c>
@@ -7571,7 +7566,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="283" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="283" spans="2:7">
       <c r="B283" t="s">
         <v>288</v>
       </c>
@@ -7591,7 +7586,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="284" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="284" spans="2:7">
       <c r="B284" t="s">
         <v>289</v>
       </c>
@@ -7611,7 +7606,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="285" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="285" spans="2:7">
       <c r="B285" t="s">
         <v>290</v>
       </c>
@@ -7631,7 +7626,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="286" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="286" spans="2:7">
       <c r="B286" t="s">
         <v>291</v>
       </c>
@@ -7651,7 +7646,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="287" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="287" spans="2:7">
       <c r="B287" t="s">
         <v>292</v>
       </c>
@@ -7671,7 +7666,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="288" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="288" spans="2:7">
       <c r="B288" t="s">
         <v>293</v>
       </c>
@@ -7691,7 +7686,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="289" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="289" spans="2:7">
       <c r="B289" t="s">
         <v>294</v>
       </c>
@@ -7711,7 +7706,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="290" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="290" spans="2:7">
       <c r="B290" t="s">
         <v>295</v>
       </c>
@@ -7731,7 +7726,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="291" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="291" spans="2:7">
       <c r="B291" t="s">
         <v>296</v>
       </c>
@@ -7751,7 +7746,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="292" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="292" spans="2:7">
       <c r="B292" t="s">
         <v>297</v>
       </c>
@@ -7771,7 +7766,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="293" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="293" spans="2:7">
       <c r="B293" t="s">
         <v>298</v>
       </c>
@@ -7791,7 +7786,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="294" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="294" spans="2:7">
       <c r="B294" t="s">
         <v>299</v>
       </c>
@@ -7811,7 +7806,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="295" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="295" spans="2:7">
       <c r="B295" t="s">
         <v>300</v>
       </c>
@@ -7831,7 +7826,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="296" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="296" spans="2:7">
       <c r="B296" t="s">
         <v>301</v>
       </c>
@@ -7851,7 +7846,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="297" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="297" spans="2:7">
       <c r="B297" t="s">
         <v>302</v>
       </c>
@@ -7871,7 +7866,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="298" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="298" spans="2:7">
       <c r="B298" t="s">
         <v>303</v>
       </c>
@@ -7891,7 +7886,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="299" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="299" spans="2:7">
       <c r="B299" t="s">
         <v>304</v>
       </c>
@@ -7911,7 +7906,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="300" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="300" spans="2:7">
       <c r="B300" t="s">
         <v>305</v>
       </c>
@@ -7931,7 +7926,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="301" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="301" spans="2:7">
       <c r="B301" t="s">
         <v>306</v>
       </c>
@@ -7951,7 +7946,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="302" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="302" spans="2:7">
       <c r="B302" t="s">
         <v>307</v>
       </c>
@@ -7971,7 +7966,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="303" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="303" spans="2:7">
       <c r="B303" t="s">
         <v>308</v>
       </c>
@@ -7991,7 +7986,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="304" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="304" spans="2:7">
       <c r="B304" t="s">
         <v>309</v>
       </c>
@@ -8011,7 +8006,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="305" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="305" spans="2:7">
       <c r="B305" t="s">
         <v>310</v>
       </c>
@@ -8031,7 +8026,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="306" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="306" spans="2:7">
       <c r="B306" t="s">
         <v>311</v>
       </c>
@@ -8051,7 +8046,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="307" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="307" spans="2:7">
       <c r="B307" t="s">
         <v>312</v>
       </c>
@@ -8071,7 +8066,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="308" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="308" spans="2:7">
       <c r="B308" t="s">
         <v>313</v>
       </c>
@@ -8091,7 +8086,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="309" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="309" spans="2:7">
       <c r="B309" t="s">
         <v>314</v>
       </c>
@@ -8111,7 +8106,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="310" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="310" spans="2:7">
       <c r="B310" t="s">
         <v>315</v>
       </c>
@@ -8131,7 +8126,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="311" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="311" spans="2:7">
       <c r="B311" t="s">
         <v>316</v>
       </c>
@@ -8151,7 +8146,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="312" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="312" spans="2:7">
       <c r="B312" t="s">
         <v>317</v>
       </c>
@@ -8171,7 +8166,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="313" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="313" spans="2:7">
       <c r="B313" t="s">
         <v>318</v>
       </c>
@@ -8191,7 +8186,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="314" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="314" spans="2:7">
       <c r="B314" t="s">
         <v>319</v>
       </c>
@@ -8211,7 +8206,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="315" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="315" spans="2:7">
       <c r="B315" t="s">
         <v>320</v>
       </c>
@@ -8231,7 +8226,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="316" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="316" spans="2:7">
       <c r="B316" t="s">
         <v>321</v>
       </c>
@@ -8251,7 +8246,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="317" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="317" spans="2:7">
       <c r="B317" t="s">
         <v>322</v>
       </c>
@@ -8271,7 +8266,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="318" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="318" spans="2:7">
       <c r="B318" t="s">
         <v>323</v>
       </c>
@@ -8291,7 +8286,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="319" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="319" spans="2:7">
       <c r="B319" t="s">
         <v>324</v>
       </c>
@@ -8311,7 +8306,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="320" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="320" spans="2:7">
       <c r="B320" t="s">
         <v>325</v>
       </c>
@@ -8331,7 +8326,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="321" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="321" spans="2:7">
       <c r="B321" t="s">
         <v>326</v>
       </c>
@@ -8351,7 +8346,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="322" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="322" spans="2:7">
       <c r="B322" t="s">
         <v>327</v>
       </c>
@@ -8371,7 +8366,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="323" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="323" spans="2:7">
       <c r="B323" t="s">
         <v>328</v>
       </c>
@@ -8391,7 +8386,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="324" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="324" spans="2:7">
       <c r="B324" t="s">
         <v>329</v>
       </c>
@@ -8411,7 +8406,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="325" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="325" spans="2:7">
       <c r="B325" t="s">
         <v>330</v>
       </c>
@@ -8431,7 +8426,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="326" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="326" spans="2:7">
       <c r="B326" t="s">
         <v>331</v>
       </c>
@@ -8451,7 +8446,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="327" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="327" spans="2:7">
       <c r="B327" t="s">
         <v>332</v>
       </c>
@@ -8471,7 +8466,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="328" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="328" spans="2:7">
       <c r="B328" t="s">
         <v>333</v>
       </c>
@@ -8491,7 +8486,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="329" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="329" spans="2:7">
       <c r="B329" t="s">
         <v>334</v>
       </c>
@@ -8511,7 +8506,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="330" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="330" spans="2:7">
       <c r="B330" t="s">
         <v>335</v>
       </c>
@@ -8531,7 +8526,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="331" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="331" spans="2:7">
       <c r="B331" t="s">
         <v>336</v>
       </c>
@@ -8551,7 +8546,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="332" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="332" spans="2:7">
       <c r="B332" t="s">
         <v>337</v>
       </c>
@@ -8571,7 +8566,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="333" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="333" spans="2:7">
       <c r="B333" t="s">
         <v>338</v>
       </c>
@@ -8591,7 +8586,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="334" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="334" spans="2:7">
       <c r="B334" t="s">
         <v>339</v>
       </c>
@@ -8611,7 +8606,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="335" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="335" spans="2:7">
       <c r="B335" t="s">
         <v>340</v>
       </c>
@@ -8631,7 +8626,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="336" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="336" spans="2:7">
       <c r="B336" t="s">
         <v>341</v>
       </c>
@@ -8651,7 +8646,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="337" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="337" spans="2:7">
       <c r="B337" t="s">
         <v>342</v>
       </c>
@@ -8671,7 +8666,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="338" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="338" spans="2:7">
       <c r="B338" t="s">
         <v>343</v>
       </c>
@@ -8691,7 +8686,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="339" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="339" spans="2:7">
       <c r="B339" t="s">
         <v>344</v>
       </c>
@@ -8711,7 +8706,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="340" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="340" spans="2:7">
       <c r="B340" t="s">
         <v>345</v>
       </c>
@@ -8731,7 +8726,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="341" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="341" spans="2:7">
       <c r="B341" t="s">
         <v>346</v>
       </c>
@@ -8751,7 +8746,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="342" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="342" spans="2:7">
       <c r="B342" t="s">
         <v>347</v>
       </c>
@@ -8771,7 +8766,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="343" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="343" spans="2:7">
       <c r="B343" t="s">
         <v>348</v>
       </c>
@@ -8791,7 +8786,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="344" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="344" spans="2:7">
       <c r="B344" t="s">
         <v>349</v>
       </c>
@@ -8811,7 +8806,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="345" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="345" spans="2:7">
       <c r="B345" t="s">
         <v>350</v>
       </c>
@@ -8831,7 +8826,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="346" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="346" spans="2:7">
       <c r="B346" t="s">
         <v>351</v>
       </c>
@@ -8851,7 +8846,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="347" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="347" spans="2:7">
       <c r="B347" t="s">
         <v>352</v>
       </c>
@@ -8871,7 +8866,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="348" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="348" spans="2:7">
       <c r="B348" t="s">
         <v>353</v>
       </c>
@@ -8891,7 +8886,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="349" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="349" spans="2:7">
       <c r="B349" t="s">
         <v>354</v>
       </c>
@@ -8911,7 +8906,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="350" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="350" spans="2:7">
       <c r="B350" t="s">
         <v>355</v>
       </c>
@@ -8931,7 +8926,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="351" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="351" spans="2:7">
       <c r="B351" t="s">
         <v>356</v>
       </c>
@@ -8951,7 +8946,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="352" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="352" spans="2:7">
       <c r="B352" t="s">
         <v>357</v>
       </c>
@@ -8971,7 +8966,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="353" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="353" spans="2:7">
       <c r="B353" t="s">
         <v>358</v>
       </c>
@@ -8991,7 +8986,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="354" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="354" spans="2:7">
       <c r="B354" t="s">
         <v>359</v>
       </c>
@@ -9011,7 +9006,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="355" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="355" spans="2:7">
       <c r="B355" t="s">
         <v>360</v>
       </c>
@@ -9031,7 +9026,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="356" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="356" spans="2:7">
       <c r="B356" t="s">
         <v>361</v>
       </c>
@@ -9051,7 +9046,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="357" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="357" spans="2:7">
       <c r="B357" t="s">
         <v>362</v>
       </c>
@@ -9071,7 +9066,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="358" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="358" spans="2:7">
       <c r="B358" t="s">
         <v>363</v>
       </c>
@@ -9091,7 +9086,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="359" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="359" spans="2:7">
       <c r="B359" t="s">
         <v>364</v>
       </c>
@@ -9111,7 +9106,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="360" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="360" spans="2:7">
       <c r="B360" t="s">
         <v>365</v>
       </c>
@@ -9131,7 +9126,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="361" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="361" spans="2:7">
       <c r="B361" t="s">
         <v>366</v>
       </c>
@@ -9151,7 +9146,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="362" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="362" spans="2:7">
       <c r="B362" t="s">
         <v>367</v>
       </c>
@@ -9171,7 +9166,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="363" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="363" spans="2:7">
       <c r="B363" t="s">
         <v>368</v>
       </c>
@@ -9191,7 +9186,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="364" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="364" spans="2:7">
       <c r="B364" t="s">
         <v>369</v>
       </c>
@@ -9211,7 +9206,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="365" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="365" spans="2:7">
       <c r="B365" t="s">
         <v>370</v>
       </c>
@@ -9231,7 +9226,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="366" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="366" spans="2:7">
       <c r="B366" t="s">
         <v>371</v>
       </c>
@@ -9251,7 +9246,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="367" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="367" spans="2:7">
       <c r="B367" t="s">
         <v>372</v>
       </c>
@@ -9271,7 +9266,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="368" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="368" spans="2:7">
       <c r="B368" t="s">
         <v>373</v>
       </c>
@@ -9291,7 +9286,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="369" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="369" spans="2:7">
       <c r="B369" t="s">
         <v>374</v>
       </c>
@@ -9311,7 +9306,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="370" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="370" spans="2:7">
       <c r="B370" t="s">
         <v>375</v>
       </c>
@@ -9331,7 +9326,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="371" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="371" spans="2:7">
       <c r="B371" t="s">
         <v>376</v>
       </c>
@@ -9351,7 +9346,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="372" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="372" spans="2:7">
       <c r="B372" t="s">
         <v>377</v>
       </c>
@@ -9371,7 +9366,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="373" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="373" spans="2:7">
       <c r="B373" t="s">
         <v>378</v>
       </c>
@@ -9391,7 +9386,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="374" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="374" spans="2:7">
       <c r="B374" t="s">
         <v>379</v>
       </c>
@@ -9411,7 +9406,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="375" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="375" spans="2:7">
       <c r="B375" t="s">
         <v>380</v>
       </c>
@@ -9431,7 +9426,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="376" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="376" spans="2:7">
       <c r="B376" t="s">
         <v>381</v>
       </c>
@@ -9451,7 +9446,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="377" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="377" spans="2:7">
       <c r="B377" t="s">
         <v>382</v>
       </c>
@@ -9471,7 +9466,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="378" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="378" spans="2:7">
       <c r="B378" t="s">
         <v>383</v>
       </c>
@@ -9491,7 +9486,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="379" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="379" spans="2:7">
       <c r="B379" t="s">
         <v>384</v>
       </c>
@@ -9511,7 +9506,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="380" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="380" spans="2:7">
       <c r="B380" t="s">
         <v>385</v>
       </c>
@@ -9531,7 +9526,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="381" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="381" spans="2:7">
       <c r="B381" t="s">
         <v>386</v>
       </c>
@@ -9551,7 +9546,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="382" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="382" spans="2:7">
       <c r="B382" t="s">
         <v>387</v>
       </c>
@@ -9571,7 +9566,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="383" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="383" spans="2:7">
       <c r="B383" t="s">
         <v>388</v>
       </c>
@@ -9591,7 +9586,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="384" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="384" spans="2:7">
       <c r="B384" t="s">
         <v>389</v>
       </c>
@@ -9611,7 +9606,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="385" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="385" spans="2:7">
       <c r="B385" t="s">
         <v>390</v>
       </c>
@@ -9631,7 +9626,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="386" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="386" spans="2:7">
       <c r="B386" t="s">
         <v>391</v>
       </c>
@@ -9651,7 +9646,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="387" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="387" spans="2:7">
       <c r="B387" t="s">
         <v>392</v>
       </c>
@@ -9671,7 +9666,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="388" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="388" spans="2:7">
       <c r="B388" t="s">
         <v>393</v>
       </c>
@@ -9691,7 +9686,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="389" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="389" spans="2:7">
       <c r="B389" t="s">
         <v>394</v>
       </c>
@@ -9711,7 +9706,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="390" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="390" spans="2:7">
       <c r="B390" t="s">
         <v>395</v>
       </c>
@@ -9731,7 +9726,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="391" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="391" spans="2:7">
       <c r="B391" t="s">
         <v>396</v>
       </c>
@@ -9751,7 +9746,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="392" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="392" spans="2:7">
       <c r="B392" t="s">
         <v>397</v>
       </c>
@@ -9771,7 +9766,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="393" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="393" spans="2:7">
       <c r="B393" t="s">
         <v>398</v>
       </c>
@@ -9791,7 +9786,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="394" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="394" spans="2:7">
       <c r="B394" t="s">
         <v>399</v>
       </c>
@@ -9811,7 +9806,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="395" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="395" spans="2:7">
       <c r="B395" t="s">
         <v>400</v>
       </c>
@@ -9831,7 +9826,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="396" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="396" spans="2:7">
       <c r="B396" t="s">
         <v>401</v>
       </c>
@@ -9851,7 +9846,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="397" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="397" spans="2:7">
       <c r="B397" t="s">
         <v>402</v>
       </c>
@@ -9871,7 +9866,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="398" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="398" spans="2:7">
       <c r="B398" t="s">
         <v>403</v>
       </c>
@@ -9891,7 +9886,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="399" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="399" spans="2:7">
       <c r="B399" t="s">
         <v>404</v>
       </c>
@@ -9911,7 +9906,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="400" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="400" spans="2:7">
       <c r="B400" t="s">
         <v>405</v>
       </c>
@@ -9931,7 +9926,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="401" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="401" spans="2:7">
       <c r="B401" t="s">
         <v>406</v>
       </c>
@@ -9951,7 +9946,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="402" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="402" spans="2:7">
       <c r="B402" t="s">
         <v>407</v>
       </c>
@@ -9971,7 +9966,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="403" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="403" spans="2:7">
       <c r="B403" t="s">
         <v>408</v>
       </c>
@@ -9991,7 +9986,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="404" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="404" spans="2:7">
       <c r="B404" t="s">
         <v>409</v>
       </c>
@@ -10011,7 +10006,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="405" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="405" spans="2:7">
       <c r="B405" t="s">
         <v>410</v>
       </c>
@@ -10031,7 +10026,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="406" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="406" spans="2:7">
       <c r="B406" t="s">
         <v>411</v>
       </c>
@@ -10051,7 +10046,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="407" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="407" spans="2:7">
       <c r="B407" t="s">
         <v>412</v>
       </c>
@@ -10071,7 +10066,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="408" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="408" spans="2:7">
       <c r="B408" t="s">
         <v>413</v>
       </c>
@@ -10091,7 +10086,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="409" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="409" spans="2:7">
       <c r="B409" t="s">
         <v>414</v>
       </c>
@@ -10111,7 +10106,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="410" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="410" spans="2:7">
       <c r="B410" t="s">
         <v>415</v>
       </c>
@@ -10131,7 +10126,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="411" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="411" spans="2:7">
       <c r="B411" t="s">
         <v>416</v>
       </c>
@@ -10151,7 +10146,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="412" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="412" spans="2:7">
       <c r="B412" t="s">
         <v>417</v>
       </c>
@@ -10171,7 +10166,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="413" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="413" spans="2:7">
       <c r="B413" t="s">
         <v>418</v>
       </c>
@@ -10191,7 +10186,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="414" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="414" spans="2:7">
       <c r="B414" t="s">
         <v>419</v>
       </c>
@@ -10211,7 +10206,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="415" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="415" spans="2:7">
       <c r="B415" t="s">
         <v>420</v>
       </c>
@@ -10231,7 +10226,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="416" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="416" spans="2:7">
       <c r="B416" t="s">
         <v>421</v>
       </c>
@@ -10251,7 +10246,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="417" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="417" spans="2:7">
       <c r="B417" t="s">
         <v>422</v>
       </c>
@@ -10271,7 +10266,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="418" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="418" spans="2:7">
       <c r="B418" t="s">
         <v>423</v>
       </c>
@@ -10291,7 +10286,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="419" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="419" spans="2:7">
       <c r="B419" t="s">
         <v>424</v>
       </c>
@@ -10311,7 +10306,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="420" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="420" spans="2:7">
       <c r="B420" t="s">
         <v>425</v>
       </c>
@@ -10331,7 +10326,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="421" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="421" spans="2:7">
       <c r="B421" t="s">
         <v>426</v>
       </c>
@@ -10351,7 +10346,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="422" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="422" spans="2:7">
       <c r="B422" t="s">
         <v>427</v>
       </c>
@@ -10371,7 +10366,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="423" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="423" spans="2:7">
       <c r="B423" t="s">
         <v>428</v>
       </c>
@@ -10391,7 +10386,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="424" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="424" spans="2:7">
       <c r="B424" t="s">
         <v>429</v>
       </c>
@@ -10411,7 +10406,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="425" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="425" spans="2:7">
       <c r="B425" t="s">
         <v>430</v>
       </c>
@@ -10431,7 +10426,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="426" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="426" spans="2:7">
       <c r="B426" t="s">
         <v>431</v>
       </c>
@@ -10451,7 +10446,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="427" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="427" spans="2:7">
       <c r="B427" t="s">
         <v>432</v>
       </c>
@@ -10471,7 +10466,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="428" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="428" spans="2:7">
       <c r="B428" t="s">
         <v>433</v>
       </c>
@@ -10491,7 +10486,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="429" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="429" spans="2:7">
       <c r="B429" t="s">
         <v>434</v>
       </c>
@@ -10511,7 +10506,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="430" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="430" spans="2:7">
       <c r="B430" t="s">
         <v>435</v>
       </c>
@@ -10531,7 +10526,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="431" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="431" spans="2:7">
       <c r="B431" t="s">
         <v>436</v>
       </c>
@@ -10551,7 +10546,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="432" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="432" spans="2:7">
       <c r="B432" t="s">
         <v>437</v>
       </c>
@@ -10571,7 +10566,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="433" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="433" spans="2:7">
       <c r="B433" t="s">
         <v>438</v>
       </c>
@@ -10591,7 +10586,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="434" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="434" spans="2:7">
       <c r="B434" t="s">
         <v>439</v>
       </c>
@@ -10611,7 +10606,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="435" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="435" spans="2:7">
       <c r="B435" t="s">
         <v>440</v>
       </c>
@@ -10631,7 +10626,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="436" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="436" spans="2:7">
       <c r="B436" t="s">
         <v>441</v>
       </c>
@@ -10651,7 +10646,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="437" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="437" spans="2:7">
       <c r="B437" t="s">
         <v>442</v>
       </c>
@@ -10671,7 +10666,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="438" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="438" spans="2:7">
       <c r="B438" t="s">
         <v>443</v>
       </c>
@@ -10691,7 +10686,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="439" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="439" spans="2:7">
       <c r="B439" t="s">
         <v>444</v>
       </c>
@@ -10711,7 +10706,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="440" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="440" spans="2:7">
       <c r="B440" t="s">
         <v>445</v>
       </c>
@@ -10731,7 +10726,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="441" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="441" spans="2:7">
       <c r="B441" t="s">
         <v>446</v>
       </c>
@@ -10751,7 +10746,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="442" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="442" spans="2:7">
       <c r="B442" t="s">
         <v>447</v>
       </c>
@@ -10771,7 +10766,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="443" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="443" spans="2:7">
       <c r="B443" t="s">
         <v>448</v>
       </c>
@@ -10791,7 +10786,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="444" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="444" spans="2:7">
       <c r="B444" t="s">
         <v>449</v>
       </c>
@@ -10811,7 +10806,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="445" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="445" spans="2:7">
       <c r="B445" t="s">
         <v>450</v>
       </c>
@@ -10831,7 +10826,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="446" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="446" spans="2:7">
       <c r="B446" t="s">
         <v>451</v>
       </c>
@@ -10851,7 +10846,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="447" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="447" spans="2:7">
       <c r="B447" t="s">
         <v>452</v>
       </c>
@@ -10871,7 +10866,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="448" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="448" spans="2:7">
       <c r="B448" t="s">
         <v>453</v>
       </c>
@@ -10891,7 +10886,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="449" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="449" spans="2:7">
       <c r="B449" t="s">
         <v>454</v>
       </c>
@@ -10911,7 +10906,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="450" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="450" spans="2:7">
       <c r="B450" t="s">
         <v>455</v>
       </c>
@@ -10931,7 +10926,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="451" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="451" spans="2:7">
       <c r="B451" t="s">
         <v>456</v>
       </c>
@@ -10951,7 +10946,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="452" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="452" spans="2:7">
       <c r="B452" t="s">
         <v>457</v>
       </c>
@@ -10971,7 +10966,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="453" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="453" spans="2:7">
       <c r="B453" t="s">
         <v>458</v>
       </c>
@@ -10991,7 +10986,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="454" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="454" spans="2:7">
       <c r="B454" t="s">
         <v>459</v>
       </c>
@@ -11011,7 +11006,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="455" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="455" spans="2:7">
       <c r="B455" t="s">
         <v>460</v>
       </c>
@@ -11031,7 +11026,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="456" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="456" spans="2:7">
       <c r="B456" t="s">
         <v>461</v>
       </c>
@@ -11051,7 +11046,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="457" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="457" spans="2:7">
       <c r="B457" t="s">
         <v>462</v>
       </c>
@@ -11071,7 +11066,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="458" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="458" spans="2:7">
       <c r="B458" t="s">
         <v>463</v>
       </c>
@@ -11091,7 +11086,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="459" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="459" spans="2:7">
       <c r="B459" t="s">
         <v>464</v>
       </c>
@@ -11111,7 +11106,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="460" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="460" spans="2:7">
       <c r="B460" t="s">
         <v>465</v>
       </c>
@@ -11131,7 +11126,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="461" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="461" spans="2:7">
       <c r="B461" t="s">
         <v>466</v>
       </c>
@@ -11151,7 +11146,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="462" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="462" spans="2:7">
       <c r="B462" t="s">
         <v>467</v>
       </c>
@@ -11171,7 +11166,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="463" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="463" spans="2:7">
       <c r="B463" t="s">
         <v>468</v>
       </c>
@@ -11191,7 +11186,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="464" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="464" spans="2:7">
       <c r="B464" t="s">
         <v>469</v>
       </c>
@@ -11211,7 +11206,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="465" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="465" spans="2:7">
       <c r="B465" t="s">
         <v>470</v>
       </c>
@@ -11231,7 +11226,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="466" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="466" spans="2:7">
       <c r="B466" t="s">
         <v>471</v>
       </c>
@@ -11251,7 +11246,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="467" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="467" spans="2:7">
       <c r="B467" t="s">
         <v>472</v>
       </c>
@@ -11271,7 +11266,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="468" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="468" spans="2:7">
       <c r="B468" t="s">
         <v>473</v>
       </c>
@@ -11291,7 +11286,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="469" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="469" spans="2:7">
       <c r="B469" t="s">
         <v>474</v>
       </c>
@@ -11311,7 +11306,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="470" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="470" spans="2:7">
       <c r="B470" t="s">
         <v>475</v>
       </c>
@@ -11331,7 +11326,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="471" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="471" spans="2:7">
       <c r="B471" t="s">
         <v>476</v>
       </c>
@@ -11351,7 +11346,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="472" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="472" spans="2:7">
       <c r="B472" t="s">
         <v>477</v>
       </c>
@@ -11371,7 +11366,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="473" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="473" spans="2:7">
       <c r="B473" t="s">
         <v>478</v>
       </c>
@@ -11397,326 +11392,268 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A62"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:1" ht="20.25">
       <c r="A1" s="3" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:1" ht="20.25">
       <c r="A2" s="3" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:1" ht="20.25">
       <c r="A3" s="3" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:1" ht="20.25">
       <c r="A4" s="3" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:1" ht="20.25">
       <c r="A5" s="3" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:1" ht="20.25">
       <c r="A6" s="3" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:1" ht="20.25">
       <c r="A7" s="3" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:1" ht="20.25">
       <c r="A8" s="3" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:1" ht="20.25">
       <c r="A9" s="3" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:1" ht="20.25">
       <c r="A10" s="3" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:1" ht="20.25">
       <c r="A11" s="3" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:1" ht="20.25">
       <c r="A12" s="3" t="s">
         <v>490</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:1" ht="20.25">
       <c r="A13" s="3" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:1" ht="20.25">
       <c r="A14" s="3" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:1" ht="20.25">
       <c r="A15" s="3" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:1" ht="20.25">
       <c r="A16" s="3" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:1" ht="20.25">
       <c r="A17" s="3" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:1" ht="20.25">
       <c r="A18" s="3" t="s">
         <v>496</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:1" ht="20.25">
       <c r="A19" s="3" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:1" ht="20.25">
       <c r="A20" s="3" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:1" ht="20.25">
       <c r="A21" s="3" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:1" ht="20.25">
       <c r="A22" s="3" t="s">
         <v>500</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:1" ht="20.25">
       <c r="A23" s="3" t="s">
         <v>501</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:1" ht="20.25">
       <c r="A24" s="3" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="25" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:1" ht="20.25">
       <c r="A25" s="3" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="26" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:1" ht="20.25">
       <c r="A26" s="3" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="27" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:1" ht="20.25">
       <c r="A27" s="3" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="28" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:1" ht="20.25">
       <c r="A28" s="3" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="29" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:1" ht="20.25">
       <c r="A29" s="3" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="30" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:1" ht="20.25">
       <c r="A30" s="3" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="31" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:1" ht="20.25">
       <c r="A31" s="3" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="32" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:1" ht="20.25">
       <c r="A32" s="3" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="33" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:1" ht="20.25">
       <c r="A33" s="3" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="34" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:1" ht="20.25">
       <c r="A34" s="3" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="35" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:1" ht="20.25">
       <c r="A35" s="3" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="36" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:1" ht="20.25">
       <c r="A36" s="3" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="37" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:1" ht="20.25">
       <c r="A37" s="3" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="38" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:1" ht="20.25">
       <c r="A38" s="3" t="s">
         <v>516</v>
       </c>
     </row>
-    <row r="39" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:1" ht="20.25">
       <c r="A39" s="3" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="40" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:1" ht="20.25">
       <c r="A40" s="3" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="41" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:1" ht="20.25">
       <c r="A41" s="3" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="42" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:1" ht="20.25">
       <c r="A42" s="3" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="43" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:1" ht="20.25">
       <c r="A43" s="3" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="44" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:1" ht="20.25">
       <c r="A44" s="3" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="45" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:1" ht="20.25">
       <c r="A45" s="3" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="46" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:1" ht="20.25">
       <c r="A46" s="3" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="47" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:1" ht="20.25">
       <c r="A47" s="3" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="48" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:1" ht="20.25">
       <c r="A48" s="3" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="49" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:1" ht="20.25">
       <c r="A49" s="3" t="s">
         <v>527</v>
       </c>
     </row>
-    <row r="50" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:1" ht="20.25">
       <c r="A50" s="3" t="s">
         <v>528</v>
       </c>
     </row>
-    <row r="51" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:1" ht="20.25">
       <c r="A51" s="3" t="s">
         <v>529</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>